<commit_message>
Add logfile to project
</commit_message>
<xml_diff>
--- a/dane.xlsx
+++ b/dane.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,13 +488,13 @@
         <v>1.5</v>
       </c>
       <c r="E2" t="n">
-        <v>2500</v>
+        <v>9500</v>
       </c>
       <c r="F2" t="n">
-        <v>6500</v>
+        <v>20250</v>
       </c>
       <c r="G2" t="n">
-        <v>-4000</v>
+        <v>-10750</v>
       </c>
     </row>
     <row r="3">
@@ -517,6 +517,27 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sausage</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>150</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>55</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>